<commit_message>
update README.md and modify RTK ports
</commit_message>
<xml_diff>
--- a/Project Outputs for AdaptWingPower/AdaptWingPower.xlsx
+++ b/Project Outputs for AdaptWingPower/AdaptWingPower.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\17929\Desktop\AdaptWing\AdaptWingPower\Project Outputs for AdaptWingPower\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1AE6CD8C-FBE1-4EF0-89C7-1FC405E4FB58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F263A1A-A43C-4B02-BAB8-580F0D1BDCC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25420" yWindow="-220" windowWidth="25780" windowHeight="15350" xr2:uid="{52E42022-4740-4608-BBBE-58BD4EE99C38}"/>
+    <workbookView xWindow="25490" yWindow="-980" windowWidth="25820" windowHeight="16220" xr2:uid="{52E42022-4740-4608-BBBE-58BD4EE99C38}"/>
   </bookViews>
   <sheets>
     <sheet name="AdaptWingPower" sheetId="1" r:id="rId1"/>
@@ -279,7 +279,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -289,6 +289,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD3D3D3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -322,7 +328,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -336,6 +342,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -654,11 +669,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{190486B7-A638-4EF7-A4F7-2316536107B6}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="6" width="17.375" customWidth="1"/>
+    <col min="1" max="3" width="17.375" customWidth="1"/>
+    <col min="4" max="4" width="29.25" customWidth="1"/>
+    <col min="5" max="6" width="17.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -717,59 +736,61 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="F4" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
+      <c r="B5" s="6"/>
+      <c r="C5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="F5" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="2" t="s">
+      <c r="B6" s="6">
+        <v>3</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="6">
         <v>1</v>
       </c>
     </row>
@@ -793,41 +814,41 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="2" t="s">
+      <c r="B8" s="6"/>
+      <c r="C8" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="F8" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="6">
         <v>2</v>
       </c>
     </row>
@@ -849,41 +870,41 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+    <row r="11" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="2" t="s">
+      <c r="B11" s="6"/>
+      <c r="C11" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F11" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+      <c r="F11" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="6">
         <v>1</v>
       </c>
     </row>
@@ -935,21 +956,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+    <row r="16" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="2" t="s">
+      <c r="B16" s="6"/>
+      <c r="C16" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F16" s="6">
         <v>1</v>
       </c>
     </row>
@@ -993,23 +1014,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
+    <row r="19" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F19" s="6">
         <v>1</v>
       </c>
     </row>
@@ -1053,23 +1074,23 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
+    <row r="22" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E22" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="F22" s="1">
+      <c r="F22" s="6">
         <v>1</v>
       </c>
     </row>
@@ -1093,43 +1114,43 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
+    <row r="24" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E24" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="F24" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
+      <c r="F24" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D25" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="E25" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="F25" s="1">
+      <c r="F25" s="6">
         <v>1</v>
       </c>
     </row>

</xml_diff>